<commit_message>
fertiges Pflichtenheft, Meilenstein 5, Tagebuch bis 21.01.15
</commit_message>
<xml_diff>
--- a/AKTUELL/Sopra Tagebuch.xlsx
+++ b/AKTUELL/Sopra Tagebuch.xlsx
@@ -175,6 +175,81 @@
     <t>Besprechung und Abschluss von Meilenstein 2</t>
   </si>
   <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Meilenstein 3: Alles + Neuformatierung, Neuer Table of Contents</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Verbesserung des Pflichtenhefts</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Verbesserung des Pflichtenhefts</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Verbesserung des Pflichtenhefts und Meilenstein 4</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Besprechung von Meilenstein 5</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Meilenstein 5</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Meilenstein 5</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Meilenstein 5</t>
+  </si>
+  <si>
     <t>Gesamt:</t>
   </si>
 </sst>
@@ -188,7 +263,7 @@
     <numFmt numFmtId="166" formatCode="hh:mm"/>
     <numFmt numFmtId="167" formatCode="d/\ mmm"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="10.0"/>
       <name val="Arial"/>
@@ -228,6 +303,9 @@
       <name val="Arial"/>
     </font>
     <font/>
+    <font>
+      <sz val="10.0"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -237,7 +315,7 @@
       <patternFill patternType="lightGray"/>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -392,6 +470,14 @@
       <bottom/>
     </border>
     <border>
+      <left/>
+      <right style="dotted">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
@@ -443,7 +529,7 @@
   <cellStyleXfs count="1">
     <xf fillId="0" numFmtId="0" borderId="0" fontId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="68">
     <xf fillId="0" numFmtId="0" borderId="0" fontId="0"/>
     <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="1">
       <alignment horizontal="center"/>
@@ -563,19 +649,61 @@
     </xf>
     <xf applyBorder="1" fillId="0" xfId="0" numFmtId="0" borderId="12" applyFont="1" fontId="7"/>
     <xf applyBorder="1" fillId="0" xfId="0" numFmtId="0" borderId="13" applyFont="1" fontId="7"/>
-    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="165" borderId="12" applyFont="1" fontId="6" applyNumberFormat="1">
-      <alignment vertical="center" horizontal="center" wrapText="1"/>
+    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="166" borderId="1" applyFont="1" fontId="6" applyNumberFormat="1">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="165" borderId="12" applyFont="1" fontId="8" applyNumberFormat="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="166" borderId="1" applyFont="1" fontId="8" applyNumberFormat="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="20" borderId="13" applyFont="1" fontId="8" applyNumberFormat="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="8">
+      <alignment/>
+    </xf>
+    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="8">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="13" applyFont="1" fontId="8">
+      <alignment/>
+    </xf>
+    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="164" borderId="1" applyFont="1" fontId="8" applyNumberFormat="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="164" borderId="16" applyFont="1" fontId="8" applyNumberFormat="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="164" borderId="13" applyFont="1" fontId="8" applyNumberFormat="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="13" applyFont="1" fontId="8">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="8">
+      <alignment/>
+    </xf>
+    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="165" borderId="12" applyFont="1" fontId="8" applyNumberFormat="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="166" borderId="1" applyFont="1" fontId="8" applyNumberFormat="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="20" borderId="13" applyFont="1" fontId="8" applyNumberFormat="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="13" applyFont="1" fontId="8">
+      <alignment horizontal="left"/>
     </xf>
     <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="13" applyFont="1" fontId="6">
       <alignment vertical="center" horizontal="left"/>
     </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="167" borderId="16" applyFont="1" fontId="3" applyNumberFormat="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="17" applyFont="1" fontId="6">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="164" borderId="16" applyFont="1" fontId="6" applyNumberFormat="1">
+    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="167" borderId="17" applyFont="1" fontId="3" applyNumberFormat="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="18" applyFont="1" fontId="6">
       <alignment horizontal="center"/>
     </xf>
     <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="164" borderId="17" applyFont="1" fontId="6" applyNumberFormat="1">
@@ -584,7 +712,10 @@
     <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="164" borderId="18" applyFont="1" fontId="6" applyNumberFormat="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="19" applyFont="1" fontId="6">
+    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="164" borderId="19" applyFont="1" fontId="6" applyNumberFormat="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="20" applyFont="1" fontId="6">
       <alignment horizontal="left"/>
     </xf>
     <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="167" borderId="1" applyFont="1" fontId="1" applyNumberFormat="1">
@@ -602,14 +733,14 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/worksheetdrawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram">
   <xdr:absoluteAnchor>
     <xdr:pos y="0" x="6400800"/>
     <xdr:ext cy="381000" cx="0"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image00.png"/>
+        <xdr:cNvPr id="0" name="image03.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -635,7 +766,7 @@
     <xdr:ext cy="38100" cx="2247900"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image02.png"/>
+        <xdr:cNvPr id="0" name="image01.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -661,7 +792,7 @@
     <xdr:ext cy="38100" cx="695325"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image04.png"/>
+        <xdr:cNvPr id="0" name="image05.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -687,7 +818,7 @@
     <xdr:ext cy="361950" cx="2867025"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image03.png"/>
+        <xdr:cNvPr id="0" name="image00.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -713,7 +844,7 @@
     <xdr:ext cy="361950" cx="1838325"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image05.png"/>
+        <xdr:cNvPr id="0" name="image04.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -739,7 +870,7 @@
     <xdr:ext cy="361950" cx="1771650"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image01.png"/>
+        <xdr:cNvPr id="0" name="image02.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1540,19 +1671,19 @@
       </c>
       <c s="26" r="F19"/>
       <c t="str" s="27" r="G19">
-        <f ref="G19:G33" t="shared" si="10">IF(ISBLANK(D19)," ",C19-B19)</f>
+        <f ref="G19:G30" t="shared" si="10">IF(ISBLANK(D19)," ",C19-B19)</f>
         <v> </v>
       </c>
       <c t="str" s="28" r="H19">
-        <f ref="H19:H33" t="shared" si="11">IF(ISBLANK(E19)," ",C19-B19)</f>
+        <f ref="H19:H30" t="shared" si="11">IF(ISBLANK(E19)," ",C19-B19)</f>
         <v>1:30</v>
       </c>
       <c t="str" s="28" r="I19">
-        <f ref="I19:I33" t="shared" si="12">IF(ISBLANK(F19)," ",C19-B19)</f>
+        <f ref="I19:I30" t="shared" si="12">IF(ISBLANK(F19)," ",C19-B19)</f>
         <v> </v>
       </c>
       <c t="str" s="29" r="J19">
-        <f ref="J19:J33" t="shared" si="13">IF(SUM(G19:I19)&gt;0,SUM(G19:I19)," ")</f>
+        <f ref="J19:J27" t="shared" si="13">IF(SUM(G19:I19)&gt;0,SUM(G19:I19)," ")</f>
         <v>1:30</v>
       </c>
       <c t="s" s="38" r="K19">
@@ -1654,29 +1785,43 @@
       <c s="31" r="U21"/>
     </row>
     <row customHeight="1" r="22" ht="12.0">
-      <c s="43" r="A22"/>
-      <c s="23" r="B22"/>
-      <c s="24" r="C22"/>
-      <c s="25" r="D22"/>
-      <c s="26" r="E22"/>
-      <c s="26" r="F22"/>
+      <c s="34" r="A22">
+        <v>41981.0</v>
+      </c>
+      <c s="35" r="B22">
+        <v>0.5833333333333334</v>
+      </c>
+      <c s="39" r="C22">
+        <v>0.75</v>
+      </c>
+      <c t="s" s="40" r="D22">
+        <v>54</v>
+      </c>
+      <c t="s" s="37" r="E22">
+        <v>55</v>
+      </c>
+      <c t="s" s="37" r="F22">
+        <v>56</v>
+      </c>
       <c t="str" s="27" r="G22">
         <f t="shared" si="10"/>
-        <v> </v>
+        <v>4:00</v>
       </c>
       <c t="str" s="28" r="H22">
         <f t="shared" si="11"/>
-        <v> </v>
+        <v>4:00</v>
       </c>
       <c t="str" s="28" r="I22">
         <f t="shared" si="12"/>
-        <v> </v>
+        <v>4:00</v>
       </c>
       <c t="str" s="29" r="J22">
         <f t="shared" si="13"/>
-        <v> </v>
-      </c>
-      <c s="32" r="K22"/>
+        <v>12:00</v>
+      </c>
+      <c t="s" s="38" r="K22">
+        <v>57</v>
+      </c>
       <c s="31" r="L22"/>
       <c s="31" r="M22"/>
       <c s="31" r="N22"/>
@@ -1689,19 +1834,27 @@
       <c s="31" r="U22"/>
     </row>
     <row customHeight="1" r="23" ht="12.0">
-      <c s="22" r="A23"/>
-      <c s="23" r="B23"/>
-      <c s="24" r="C23"/>
-      <c s="25" r="D23"/>
-      <c s="26" r="E23"/>
-      <c s="26" r="F23"/>
+      <c s="34" r="A23">
+        <v>41989.0</v>
+      </c>
+      <c s="35" r="B23">
+        <v>0.875</v>
+      </c>
+      <c s="39" r="C23">
+        <v>0.9166666666666666</v>
+      </c>
+      <c s="40" r="D23"/>
+      <c t="s" s="37" r="E23">
+        <v>58</v>
+      </c>
+      <c s="37" r="F23"/>
       <c t="str" s="27" r="G23">
         <f t="shared" si="10"/>
         <v> </v>
       </c>
       <c t="str" s="28" r="H23">
         <f t="shared" si="11"/>
-        <v> </v>
+        <v>1:00</v>
       </c>
       <c t="str" s="28" r="I23">
         <f t="shared" si="12"/>
@@ -1709,9 +1862,11 @@
       </c>
       <c t="str" s="29" r="J23">
         <f t="shared" si="13"/>
-        <v> </v>
-      </c>
-      <c s="32" r="K23"/>
+        <v>1:00</v>
+      </c>
+      <c t="s" s="38" r="K23">
+        <v>59</v>
+      </c>
       <c s="31" r="L23"/>
       <c s="31" r="M23"/>
       <c s="31" r="N23"/>
@@ -1724,15 +1879,25 @@
       <c s="31" r="U23"/>
     </row>
     <row customHeight="1" r="24" ht="12.0">
-      <c s="22" r="A24"/>
-      <c s="23" r="B24"/>
-      <c s="24" r="C24"/>
-      <c s="25" r="D24"/>
+      <c s="34" r="A24">
+        <v>41989.0</v>
+      </c>
+      <c s="43" r="B24">
+        <v>0.6666666666666666</v>
+      </c>
+      <c s="36" r="C24">
+        <v>0.75</v>
+      </c>
+      <c t="s" s="40" r="D24">
+        <v>60</v>
+      </c>
       <c s="26" r="E24"/>
-      <c s="26" r="F24"/>
+      <c t="s" s="37" r="F24">
+        <v>61</v>
+      </c>
       <c t="str" s="27" r="G24">
         <f t="shared" si="10"/>
-        <v> </v>
+        <v>2:00</v>
       </c>
       <c t="str" s="28" r="H24">
         <f t="shared" si="11"/>
@@ -1740,13 +1905,15 @@
       </c>
       <c t="str" s="28" r="I24">
         <f t="shared" si="12"/>
-        <v> </v>
+        <v>2:00</v>
       </c>
       <c t="str" s="29" r="J24">
         <f t="shared" si="13"/>
-        <v> </v>
-      </c>
-      <c s="32" r="K24"/>
+        <v>4:00</v>
+      </c>
+      <c t="s" s="38" r="K24">
+        <v>62</v>
+      </c>
       <c s="31" r="L24"/>
       <c s="31" r="M24"/>
       <c s="31" r="N24"/>
@@ -1794,29 +1961,43 @@
       <c s="31" r="U25"/>
     </row>
     <row customHeight="1" r="26" ht="12.0">
-      <c s="22" r="A26"/>
-      <c s="23" r="B26"/>
-      <c s="24" r="C26"/>
-      <c s="25" r="D26"/>
-      <c s="26" r="E26"/>
-      <c s="26" r="F26"/>
+      <c s="34" r="A26">
+        <v>42014.0</v>
+      </c>
+      <c s="43" r="B26">
+        <v>0.6666666666666666</v>
+      </c>
+      <c s="36" r="C26">
+        <v>0.75</v>
+      </c>
+      <c t="s" s="40" r="D26">
+        <v>63</v>
+      </c>
+      <c t="s" s="37" r="E26">
+        <v>64</v>
+      </c>
+      <c t="s" s="37" r="F26">
+        <v>65</v>
+      </c>
       <c t="str" s="27" r="G26">
         <f t="shared" si="10"/>
-        <v> </v>
+        <v>2:00</v>
       </c>
       <c t="str" s="28" r="H26">
         <f t="shared" si="11"/>
-        <v> </v>
+        <v>2:00</v>
       </c>
       <c t="str" s="28" r="I26">
         <f t="shared" si="12"/>
-        <v> </v>
+        <v>2:00</v>
       </c>
       <c t="str" s="29" r="J26">
         <f t="shared" si="13"/>
-        <v> </v>
-      </c>
-      <c s="32" r="K26"/>
+        <v>6:00</v>
+      </c>
+      <c t="s" s="38" r="K26">
+        <v>66</v>
+      </c>
       <c s="31" r="L26"/>
       <c s="31" r="M26"/>
       <c s="31" r="N26"/>
@@ -1829,29 +2010,43 @@
       <c s="31" r="U26"/>
     </row>
     <row customHeight="1" r="27" ht="12.0">
-      <c s="22" r="A27"/>
-      <c s="23" r="B27"/>
-      <c s="24" r="C27"/>
-      <c s="25" r="D27"/>
-      <c s="26" r="E27"/>
-      <c s="26" r="F27"/>
+      <c s="34" r="A27">
+        <v>42020.0</v>
+      </c>
+      <c s="43" r="B27">
+        <v>0.4166666666666667</v>
+      </c>
+      <c s="36" r="C27">
+        <v>0.5</v>
+      </c>
+      <c t="s" s="40" r="D27">
+        <v>67</v>
+      </c>
+      <c t="s" s="37" r="E27">
+        <v>68</v>
+      </c>
+      <c t="s" s="37" r="F27">
+        <v>69</v>
+      </c>
       <c t="str" s="27" r="G27">
         <f t="shared" si="10"/>
-        <v> </v>
+        <v>2:00</v>
       </c>
       <c t="str" s="28" r="H27">
         <f t="shared" si="11"/>
-        <v> </v>
+        <v>2:00</v>
       </c>
       <c t="str" s="28" r="I27">
         <f t="shared" si="12"/>
-        <v> </v>
+        <v>2:00</v>
       </c>
       <c t="str" s="29" r="J27">
         <f t="shared" si="13"/>
-        <v> </v>
-      </c>
-      <c s="32" r="K27"/>
+        <v>6:00</v>
+      </c>
+      <c t="s" s="38" r="K27">
+        <v>70</v>
+      </c>
       <c s="31" r="L27"/>
       <c s="31" r="M27"/>
       <c s="31" r="N27"/>
@@ -1864,144 +2059,166 @@
       <c s="31" r="U27"/>
     </row>
     <row customHeight="1" r="28" ht="12.0">
-      <c s="22" r="A28"/>
-      <c s="23" r="B28"/>
-      <c s="24" r="C28"/>
-      <c s="25" r="D28"/>
-      <c s="26" r="E28"/>
-      <c s="26" r="F28"/>
-      <c t="str" s="27" r="G28">
+      <c s="44" r="A28">
+        <v>42021.0</v>
+      </c>
+      <c s="45" r="B28">
+        <v>0.8333333333333334</v>
+      </c>
+      <c s="46" r="C28">
+        <v>0.9166666666666666</v>
+      </c>
+      <c s="47" r="D28"/>
+      <c t="s" s="48" r="E28">
+        <v>71</v>
+      </c>
+      <c s="49" r="F28"/>
+      <c t="str" s="50" r="G28">
         <f t="shared" si="10"/>
         <v> </v>
       </c>
-      <c t="str" s="28" r="H28">
+      <c t="str" s="50" r="H28">
         <f t="shared" si="11"/>
-        <v> </v>
-      </c>
-      <c t="str" s="28" r="I28">
+        <v>2:00</v>
+      </c>
+      <c t="str" s="51" r="I28">
         <f t="shared" si="12"/>
         <v> </v>
       </c>
-      <c t="str" s="29" r="J28">
-        <f t="shared" si="13"/>
-        <v> </v>
-      </c>
-      <c s="32" r="K28"/>
-      <c s="31" r="L28"/>
-      <c s="31" r="M28"/>
-      <c s="31" r="N28"/>
-      <c s="31" r="O28"/>
-      <c s="31" r="P28"/>
-      <c s="31" r="Q28"/>
-      <c s="31" r="R28"/>
-      <c s="31" r="S28"/>
-      <c s="31" r="T28"/>
-      <c s="31" r="U28"/>
+      <c t="str" s="52" r="J28">
+        <f ref="J28:J30" t="shared" si="14">IF(SUM(G28:I28)&gt;0,SUM(G28:I28)," ")</f>
+        <v>2:00</v>
+      </c>
+      <c t="s" s="53" r="K28">
+        <v>72</v>
+      </c>
+      <c s="54" r="L28"/>
+      <c s="54" r="M28"/>
+      <c s="54" r="N28"/>
+      <c s="54" r="O28"/>
+      <c s="54" r="P28"/>
+      <c s="54" r="Q28"/>
+      <c s="54" r="R28"/>
+      <c s="54" r="S28"/>
+      <c s="54" r="T28"/>
+      <c s="54" r="U28"/>
     </row>
     <row customHeight="1" r="29" ht="12.0">
-      <c s="22" r="A29"/>
-      <c s="23" r="B29"/>
-      <c s="24" r="C29"/>
-      <c s="25" r="D29"/>
+      <c s="55" r="A29">
+        <v>42023.0</v>
+      </c>
+      <c s="56" r="B29">
+        <v>0.7083333333333334</v>
+      </c>
+      <c s="57" r="C29">
+        <v>0.7916666666666666</v>
+      </c>
+      <c t="s" s="40" r="D29">
+        <v>73</v>
+      </c>
       <c s="26" r="E29"/>
-      <c s="26" r="F29"/>
-      <c t="str" s="27" r="G29">
+      <c t="s" s="37" r="F29">
+        <v>74</v>
+      </c>
+      <c t="str" s="50" r="G29">
         <f t="shared" si="10"/>
-        <v> </v>
-      </c>
-      <c t="str" s="28" r="H29">
+        <v>2:00</v>
+      </c>
+      <c t="str" s="50" r="H29">
         <f t="shared" si="11"/>
         <v> </v>
       </c>
-      <c t="str" s="28" r="I29">
+      <c t="str" s="51" r="I29">
         <f t="shared" si="12"/>
-        <v> </v>
-      </c>
-      <c t="str" s="29" r="J29">
-        <f t="shared" si="13"/>
-        <v> </v>
-      </c>
-      <c s="32" r="K29"/>
-      <c s="31" r="L29"/>
-      <c s="31" r="M29"/>
-      <c s="31" r="N29"/>
-      <c s="31" r="O29"/>
-      <c s="31" r="P29"/>
-      <c s="31" r="Q29"/>
-      <c s="31" r="R29"/>
-      <c s="31" r="S29"/>
-      <c s="31" r="T29"/>
-      <c s="31" r="U29"/>
+        <v>2:00</v>
+      </c>
+      <c t="str" s="52" r="J29">
+        <f t="shared" si="14"/>
+        <v>4:00</v>
+      </c>
+      <c t="s" s="58" r="K29">
+        <v>75</v>
+      </c>
+      <c s="54" r="L29"/>
+      <c s="54" r="M29"/>
+      <c s="54" r="N29"/>
+      <c s="54" r="O29"/>
+      <c s="54" r="P29"/>
+      <c s="54" r="Q29"/>
+      <c s="54" r="R29"/>
+      <c s="54" r="S29"/>
+      <c s="54" r="T29"/>
+      <c s="54" r="U29"/>
     </row>
     <row customHeight="1" r="30" ht="12.0">
-      <c s="22" r="A30"/>
-      <c s="23" r="B30"/>
-      <c s="24" r="C30"/>
-      <c s="25" r="D30"/>
+      <c s="55" r="A30">
+        <v>42025.0</v>
+      </c>
+      <c s="56" r="B30">
+        <v>0.4270833333333333</v>
+      </c>
+      <c s="57" r="C30">
+        <v>0.4583333333333333</v>
+      </c>
+      <c t="s" s="40" r="D30">
+        <v>76</v>
+      </c>
       <c s="26" r="E30"/>
-      <c s="26" r="F30"/>
-      <c t="str" s="27" r="G30">
+      <c t="s" s="37" r="F30">
+        <v>77</v>
+      </c>
+      <c t="str" s="50" r="G30">
         <f t="shared" si="10"/>
-        <v> </v>
-      </c>
-      <c t="str" s="28" r="H30">
+        <v>0:45</v>
+      </c>
+      <c t="str" s="50" r="H30">
         <f t="shared" si="11"/>
         <v> </v>
       </c>
-      <c t="str" s="28" r="I30">
+      <c t="str" s="51" r="I30">
         <f t="shared" si="12"/>
-        <v> </v>
-      </c>
-      <c t="str" s="29" r="J30">
-        <f t="shared" si="13"/>
-        <v> </v>
-      </c>
-      <c s="32" r="K30"/>
-      <c s="31" r="L30"/>
-      <c s="31" r="M30"/>
-      <c s="31" r="N30"/>
-      <c s="31" r="O30"/>
-      <c s="31" r="P30"/>
-      <c s="31" r="Q30"/>
-      <c s="31" r="R30"/>
-      <c s="31" r="S30"/>
-      <c s="31" r="T30"/>
-      <c s="31" r="U30"/>
+        <v>0:45</v>
+      </c>
+      <c t="str" s="52" r="J30">
+        <f t="shared" si="14"/>
+        <v>1:30</v>
+      </c>
+      <c t="s" s="58" r="K30">
+        <v>78</v>
+      </c>
+      <c s="54" r="L30"/>
+      <c s="54" r="M30"/>
+      <c s="54" r="N30"/>
+      <c s="54" r="O30"/>
+      <c s="54" r="P30"/>
+      <c s="54" r="Q30"/>
+      <c s="54" r="R30"/>
+      <c s="54" r="S30"/>
+      <c s="54" r="T30"/>
+      <c s="54" r="U30"/>
     </row>
     <row customHeight="1" r="31" ht="12.0">
-      <c s="22" r="A31"/>
-      <c s="23" r="B31"/>
-      <c s="24" r="C31"/>
-      <c s="25" r="D31"/>
+      <c s="44" r="A31"/>
+      <c s="45" r="B31"/>
+      <c s="46" r="C31"/>
+      <c s="40" r="D31"/>
       <c s="26" r="E31"/>
-      <c s="26" r="F31"/>
-      <c t="str" s="27" r="G31">
-        <f t="shared" si="10"/>
-        <v> </v>
-      </c>
-      <c t="str" s="28" r="H31">
-        <f t="shared" si="11"/>
-        <v> </v>
-      </c>
-      <c t="str" s="28" r="I31">
-        <f t="shared" si="12"/>
-        <v> </v>
-      </c>
-      <c t="str" s="29" r="J31">
-        <f t="shared" si="13"/>
-        <v> </v>
-      </c>
-      <c s="32" r="K31"/>
-      <c s="31" r="L31"/>
-      <c s="31" r="M31"/>
-      <c s="31" r="N31"/>
-      <c s="31" r="O31"/>
-      <c s="31" r="P31"/>
-      <c s="31" r="Q31"/>
-      <c s="31" r="R31"/>
-      <c s="31" r="S31"/>
-      <c s="31" r="T31"/>
-      <c s="31" r="U31"/>
+      <c s="37" r="F31"/>
+      <c s="50" r="G31"/>
+      <c s="50" r="H31"/>
+      <c s="51" r="I31"/>
+      <c s="52" r="J31"/>
+      <c s="58" r="K31"/>
+      <c s="54" r="L31"/>
+      <c s="54" r="M31"/>
+      <c s="54" r="N31"/>
+      <c s="54" r="O31"/>
+      <c s="54" r="P31"/>
+      <c s="54" r="Q31"/>
+      <c s="54" r="R31"/>
+      <c s="54" r="S31"/>
+      <c s="54" r="T31"/>
+      <c s="54" r="U31"/>
     </row>
     <row customHeight="1" r="32" ht="12.0">
       <c s="22" r="A32"/>
@@ -2011,19 +2228,19 @@
       <c s="26" r="E32"/>
       <c s="26" r="F32"/>
       <c t="str" s="27" r="G32">
-        <f t="shared" si="10"/>
+        <f ref="G32:G33" t="shared" si="15">IF(ISBLANK(D32)," ",C32-B32)</f>
         <v> </v>
       </c>
       <c t="str" s="28" r="H32">
-        <f t="shared" si="11"/>
+        <f ref="H32:H33" t="shared" si="16">IF(ISBLANK(E32)," ",C32-B32)</f>
         <v> </v>
       </c>
       <c t="str" s="28" r="I32">
-        <f t="shared" si="12"/>
+        <f ref="I32:I33" t="shared" si="17">IF(ISBLANK(F32)," ",C32-B32)</f>
         <v> </v>
       </c>
       <c t="str" s="29" r="J32">
-        <f t="shared" si="13"/>
+        <f ref="J32:J33" t="shared" si="18">IF(SUM(G32:I32)&gt;0,SUM(G32:I32)," ")</f>
         <v> </v>
       </c>
       <c s="32" r="K32"/>
@@ -2046,19 +2263,19 @@
       <c s="26" r="E33"/>
       <c s="26" r="F33"/>
       <c t="str" s="27" r="G33">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v> </v>
       </c>
       <c t="str" s="28" r="H33">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v> </v>
       </c>
       <c t="str" s="28" r="I33">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v> </v>
       </c>
       <c t="str" s="29" r="J33">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v> </v>
       </c>
       <c s="32" r="K33"/>
@@ -2104,19 +2321,19 @@
       <c s="26" r="E35"/>
       <c s="26" r="F35"/>
       <c t="str" s="27" r="G35">
-        <f ref="G35:G40" t="shared" si="14">IF(ISBLANK(D35)," ",C35-B35)</f>
+        <f ref="G35:G40" t="shared" si="19">IF(ISBLANK(D35)," ",C35-B35)</f>
         <v> </v>
       </c>
       <c t="str" s="28" r="H35">
-        <f ref="H35:H40" t="shared" si="15">IF(ISBLANK(E35)," ",C35-B35)</f>
+        <f ref="H35:H40" t="shared" si="20">IF(ISBLANK(E35)," ",C35-B35)</f>
         <v> </v>
       </c>
       <c t="str" s="28" r="I35">
-        <f ref="I35:I40" t="shared" si="16">IF(ISBLANK(F35)," ",C35-B35)</f>
+        <f ref="I35:I40" t="shared" si="21">IF(ISBLANK(F35)," ",C35-B35)</f>
         <v> </v>
       </c>
       <c t="str" s="29" r="J35">
-        <f ref="J35:J40" t="shared" si="17">IF(SUM(G35:I35)&gt;0,SUM(G35:I35)," ")</f>
+        <f ref="J35:J40" t="shared" si="22">IF(SUM(G35:I35)&gt;0,SUM(G35:I35)," ")</f>
         <v> </v>
       </c>
       <c s="32" r="K35"/>
@@ -2139,22 +2356,22 @@
       <c s="26" r="E36"/>
       <c s="26" r="F36"/>
       <c t="str" s="27" r="G36">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v> </v>
       </c>
       <c t="str" s="28" r="H36">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v> </v>
       </c>
       <c t="str" s="28" r="I36">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v> </v>
       </c>
       <c t="str" s="29" r="J36">
-        <f t="shared" si="17"/>
-        <v> </v>
-      </c>
-      <c s="44" r="K36"/>
+        <f t="shared" si="22"/>
+        <v> </v>
+      </c>
+      <c s="59" r="K36"/>
       <c s="31" r="L36"/>
       <c s="31" r="M36"/>
       <c s="31" r="N36"/>
@@ -2174,19 +2391,19 @@
       <c s="26" r="E37"/>
       <c s="26" r="F37"/>
       <c t="str" s="27" r="G37">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v> </v>
       </c>
       <c t="str" s="28" r="H37">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v> </v>
       </c>
       <c t="str" s="28" r="I37">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v> </v>
       </c>
       <c t="str" s="29" r="J37">
-        <f t="shared" si="17"/>
+        <f t="shared" si="22"/>
         <v> </v>
       </c>
       <c s="32" r="K37"/>
@@ -2209,19 +2426,19 @@
       <c s="26" r="E38"/>
       <c s="26" r="F38"/>
       <c t="str" s="27" r="G38">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v> </v>
       </c>
       <c t="str" s="28" r="H38">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v> </v>
       </c>
       <c t="str" s="28" r="I38">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v> </v>
       </c>
       <c t="str" s="29" r="J38">
-        <f t="shared" si="17"/>
+        <f t="shared" si="22"/>
         <v> </v>
       </c>
       <c s="32" r="K38"/>
@@ -2244,19 +2461,19 @@
       <c s="26" r="E39"/>
       <c s="26" r="F39"/>
       <c t="str" s="27" r="G39">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v> </v>
       </c>
       <c t="str" s="28" r="H39">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v> </v>
       </c>
       <c t="str" s="28" r="I39">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v> </v>
       </c>
       <c t="str" s="29" r="J39">
-        <f t="shared" si="17"/>
+        <f t="shared" si="22"/>
         <v> </v>
       </c>
       <c s="32" r="K39"/>
@@ -2279,19 +2496,19 @@
       <c s="26" r="E40"/>
       <c s="26" r="F40"/>
       <c t="str" s="27" r="G40">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v> </v>
       </c>
       <c t="str" s="28" r="H40">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v> </v>
       </c>
       <c t="str" s="28" r="I40">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v> </v>
       </c>
       <c t="str" s="29" r="J40">
-        <f t="shared" si="17"/>
+        <f t="shared" si="22"/>
         <v> </v>
       </c>
       <c s="32" r="K40"/>
@@ -2307,31 +2524,31 @@
       <c s="31" r="U40"/>
     </row>
     <row customHeight="1" r="41" ht="12.0">
-      <c t="s" s="45" r="A41">
-        <v>54</v>
-      </c>
-      <c s="46" r="B41"/>
-      <c s="46" r="C41"/>
-      <c s="46" r="D41"/>
-      <c s="46" r="E41"/>
-      <c s="46" r="F41"/>
-      <c t="str" s="47" r="G41">
-        <f ref="G41:I41" t="shared" si="18">SUM(G4:G40)</f>
-        <v>22:51</v>
-      </c>
-      <c t="str" s="48" r="H41">
-        <f t="shared" si="18"/>
-        <v>23:00</v>
-      </c>
-      <c t="str" s="48" r="I41">
-        <f t="shared" si="18"/>
-        <v>22:51</v>
-      </c>
-      <c t="str" s="49" r="J41">
-        <f>SUM(J9:J40)</f>
-        <v>38:12</v>
-      </c>
-      <c s="50" r="K41"/>
+      <c t="s" s="60" r="A41">
+        <v>79</v>
+      </c>
+      <c s="61" r="B41"/>
+      <c s="61" r="C41"/>
+      <c s="61" r="D41"/>
+      <c s="61" r="E41"/>
+      <c s="61" r="F41"/>
+      <c t="str" s="62" r="G41">
+        <f ref="G41:J41" t="shared" si="23">SUM(G4:G40)</f>
+        <v>35:36</v>
+      </c>
+      <c t="str" s="63" r="H41">
+        <f t="shared" si="23"/>
+        <v>34:00</v>
+      </c>
+      <c t="str" s="63" r="I41">
+        <f t="shared" si="23"/>
+        <v>35:36</v>
+      </c>
+      <c t="str" s="64" r="J41">
+        <f t="shared" si="23"/>
+        <v>105:12</v>
+      </c>
+      <c s="65" r="K41"/>
       <c s="6" r="L41"/>
       <c s="6" r="M41"/>
       <c s="6" r="N41"/>
@@ -2344,7 +2561,7 @@
       <c s="6" r="U41"/>
     </row>
     <row customHeight="1" r="42" ht="12.0">
-      <c s="51" r="A42"/>
+      <c s="66" r="A42"/>
       <c s="1" r="B42"/>
       <c s="1" r="C42"/>
       <c s="1" r="D42"/>
@@ -2354,7 +2571,7 @@
       <c s="3" r="H42"/>
       <c s="3" r="I42"/>
       <c s="3" r="J42"/>
-      <c s="52" r="K42"/>
+      <c s="67" r="K42"/>
       <c s="6" r="L42"/>
       <c s="6" r="M42"/>
       <c s="6" r="N42"/>

</xml_diff>